<commit_message>
Update logic for measure OLS granting
</commit_message>
<xml_diff>
--- a/config/SecurityAutoBuild.xlsx
+++ b/config/SecurityAutoBuild.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trinh\Downloads\Armstrong Project\SecurityAutoBuild\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3746EAE5-0206-4EA0-B4F1-EA5DA4F60506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CC77C6-3555-4EAE-BA76-6A44451546FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{BEC676D7-2196-4582-B754-27C40BA62468}"/>
+    <workbookView xWindow="2550" yWindow="2550" windowWidth="21600" windowHeight="11235" activeTab="2" xr2:uid="{BEC676D7-2196-4582-B754-27C40BA62468}"/>
   </bookViews>
   <sheets>
     <sheet name="Roles" sheetId="7" r:id="rId1"/>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="153">
   <si>
     <t>ObjectType</t>
   </si>
@@ -657,6 +657,9 @@
   </si>
   <si>
     <t>Part Performance Metrics</t>
+  </si>
+  <si>
+    <t>Budget Amt</t>
   </si>
 </sst>
 </file>
@@ -731,7 +734,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -753,6 +756,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -796,7 +805,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -851,28 +860,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2222,10 +2222,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C81C328-5EE5-4B58-AB75-C8038C0B1D0A}">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2334,7 +2334,7 @@
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="17" t="s">
         <v>151</v>
       </c>
       <c r="B6" s="17" t="s">
@@ -2357,7 +2357,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="7" t="s">
         <v>112</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -2376,7 +2376,7 @@
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="17" t="s">
         <v>151</v>
       </c>
       <c r="B8" s="17" t="s">
@@ -2842,7 +2842,7 @@
       <c r="G31" s="19"/>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="19" t="s">
         <v>138</v>
       </c>
       <c r="B32" s="19" t="s">
@@ -2858,12 +2858,12 @@
       <c r="F32" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G32" s="25" t="s">
+      <c r="G32" s="24" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="19" t="s">
         <v>138</v>
       </c>
       <c r="B33" s="19" t="s">
@@ -2879,108 +2879,108 @@
       <c r="F33" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G33" s="25" t="s">
+      <c r="G33" s="24" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
+      <c r="A34" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C34" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="26"/>
-      <c r="E34" s="27" t="s">
+      <c r="C34" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="7"/>
+      <c r="E34" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="F34" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G34" s="26"/>
+      <c r="F34" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G34" s="7"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="26" t="s">
+      <c r="A35" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C35" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26" t="s">
+      <c r="C35" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="F35" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G35" s="26"/>
+      <c r="F35" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G35" s="7"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C36" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26" t="s">
+      <c r="C36" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="F36" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G36" s="26"/>
+      <c r="F36" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G36" s="7"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="26" t="s">
+      <c r="A37" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C37" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26" t="s">
+      <c r="C37" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F37" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G37" s="26" t="s">
+      <c r="F37" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G37" s="7" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C38" s="28" t="s">
+      <c r="C38" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="E38" s="28" t="s">
+      <c r="E38" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="F38" s="28" t="s">
+      <c r="F38" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G38" s="29" t="s">
+      <c r="G38" s="25" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3023,156 +3023,156 @@
       <c r="G40" s="19"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="26" t="s">
+      <c r="A41" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B41" s="26" t="s">
+      <c r="B41" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C41" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D41" s="26"/>
-      <c r="E41" s="27" t="s">
+      <c r="C41" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="7"/>
+      <c r="E41" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="F41" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G41" s="26"/>
+      <c r="F41" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G41" s="7"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="26" t="s">
+      <c r="A42" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="26" t="s">
+      <c r="B42" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C42" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26" t="s">
+      <c r="C42" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="F42" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G42" s="26"/>
+      <c r="F42" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G42" s="7"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="26" t="s">
+      <c r="A43" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B43" s="26" t="s">
+      <c r="B43" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C43" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26" t="s">
+      <c r="C43" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F43" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G43" s="26"/>
+      <c r="F43" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G43" s="7"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="26" t="s">
+      <c r="A44" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B44" s="26" t="s">
+      <c r="B44" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C44" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26" t="s">
+      <c r="C44" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="F44" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G44" s="26"/>
+      <c r="F44" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G44" s="7"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="26" t="s">
+      <c r="A45" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B45" s="26" t="s">
+      <c r="B45" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C45" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26" t="s">
+      <c r="C45" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="F45" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G45" s="26"/>
+      <c r="F45" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G45" s="7"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="26" t="s">
+      <c r="A46" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C46" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26" t="s">
+      <c r="C46" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="F46" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G46" s="26"/>
+      <c r="F46" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G46" s="7"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="26" t="s">
+      <c r="A47" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C47" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26" t="s">
+      <c r="C47" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="F47" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G47" s="26"/>
+      <c r="F47" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G47" s="7"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="26" t="s">
+      <c r="A48" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B48" s="26" t="s">
+      <c r="B48" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C48" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26" t="s">
+      <c r="C48" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="F48" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G48" s="26"/>
+      <c r="F48" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G48" s="7"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
@@ -3306,6 +3306,25 @@
         <v>31</v>
       </c>
       <c r="G55" s="19"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B56" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="C56" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="F56" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G56" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3317,8 +3336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1424039-4C57-425F-8425-D8A336879F05}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3583,7 +3602,7 @@
       <c r="F19" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="30" t="s">
+      <c r="G19" s="26" t="s">
         <v>146</v>
       </c>
     </row>
@@ -3606,7 +3625,7 @@
       <c r="F20" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G20" s="27" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3774,11 +3793,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="beaba498-6342-4421-a18c-7bfd16d38d53" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4017,27 +4037,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="beaba498-6342-4421-a18c-7bfd16d38d53" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9805D712-353E-429A-8628-FA34CABB75D5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2275932-CD7C-4B19-A948-199D3E0E5FFC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="beaba498-6342-4421-a18c-7bfd16d38d53"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9e548fd3-f7b4-490c-9d07-36be117e6ce5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4062,9 +4072,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2275932-CD7C-4B19-A948-199D3E0E5FFC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9805D712-353E-429A-8628-FA34CABB75D5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="beaba498-6342-4421-a18c-7bfd16d38d53"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9e548fd3-f7b4-490c-9d07-36be117e6ce5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update the final version
</commit_message>
<xml_diff>
--- a/config/SecurityAutoBuild.xlsx
+++ b/config/SecurityAutoBuild.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trinh\Downloads\Armstrong Project\SecurityAutoBuild\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CC77C6-3555-4EAE-BA76-6A44451546FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79499C0D-076F-4D4F-BB2A-2C12333D9371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="2550" windowWidth="21600" windowHeight="11235" activeTab="2" xr2:uid="{BEC676D7-2196-4582-B754-27C40BA62468}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{BEC676D7-2196-4582-B754-27C40BA62468}"/>
   </bookViews>
   <sheets>
     <sheet name="Roles" sheetId="7" r:id="rId1"/>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="154">
   <si>
     <t>ObjectType</t>
   </si>
@@ -660,13 +660,16 @@
   </si>
   <si>
     <t>Budget Amt</t>
+  </si>
+  <si>
+    <t>Testing Purpose</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -723,12 +726,6 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -805,7 +802,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -867,9 +864,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2224,8 +2218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C81C328-5EE5-4B58-AB75-C8038C0B1D0A}">
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2766,42 +2760,46 @@
       <c r="G27" s="19"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B29" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7" t="s">
+      <c r="C29" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="F28" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F29" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" s="19"/>
+      <c r="F29" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
@@ -2814,8 +2812,8 @@
         <v>34</v>
       </c>
       <c r="D30" s="19"/>
-      <c r="E30" s="19" t="s">
-        <v>113</v>
+      <c r="E30" s="20" t="s">
+        <v>88</v>
       </c>
       <c r="F30" s="19" t="s">
         <v>31</v>
@@ -2824,7 +2822,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>135</v>
@@ -2834,16 +2832,16 @@
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="19" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="F31" s="19" t="s">
         <v>31</v>
       </c>
       <c r="G31" s="19"/>
     </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>135</v>
@@ -2853,14 +2851,12 @@
       </c>
       <c r="D32" s="19"/>
       <c r="E32" s="19" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="F32" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G32" s="24" t="s">
-        <v>139</v>
-      </c>
+      <c r="G32" s="19"/>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
@@ -2874,7 +2870,7 @@
       </c>
       <c r="D33" s="19"/>
       <c r="E33" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F33" s="19" t="s">
         <v>31</v>
@@ -2883,24 +2879,26 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G34" s="7"/>
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G34" s="24" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
@@ -2913,8 +2911,8 @@
         <v>34</v>
       </c>
       <c r="D35" s="7"/>
-      <c r="E35" s="7" t="s">
-        <v>113</v>
+      <c r="E35" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>31</v>
@@ -2923,7 +2921,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>140</v>
@@ -2933,7 +2931,7 @@
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>31</v>
@@ -2942,7 +2940,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>140</v>
@@ -2952,56 +2950,56 @@
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G37" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
-        <v>112</v>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>114</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="C38" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C39" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D39" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="E39" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="F38" s="17" t="s">
+      <c r="F39" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G38" s="25" t="s">
+      <c r="G39" s="25" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D39" s="19"/>
-      <c r="E39" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F39" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="G39" s="19"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
@@ -3014,32 +3012,32 @@
         <v>34</v>
       </c>
       <c r="D40" s="19"/>
-      <c r="E40" s="19" t="s">
+      <c r="E40" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G40" s="19"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="F40" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="G40" s="19"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D41" s="7"/>
-      <c r="E41" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G41" s="7"/>
+      <c r="F41" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G41" s="19"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -3052,8 +3050,8 @@
         <v>34</v>
       </c>
       <c r="D42" s="7"/>
-      <c r="E42" s="7" t="s">
-        <v>113</v>
+      <c r="E42" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>31</v>
@@ -3062,7 +3060,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>144</v>
@@ -3072,7 +3070,7 @@
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>31</v>
@@ -3081,7 +3079,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>144</v>
@@ -3091,7 +3089,7 @@
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>31</v>
@@ -3100,7 +3098,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>144</v>
@@ -3110,7 +3108,7 @@
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="7" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>31</v>
@@ -3119,7 +3117,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>144</v>
@@ -3129,7 +3127,7 @@
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>31</v>
@@ -3148,7 +3146,7 @@
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="7" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="F47" s="7" t="s">
         <v>31</v>
@@ -3167,31 +3165,31 @@
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G48" s="7"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="F48" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G48" s="7"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="B49" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="C49" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D49" s="19"/>
-      <c r="E49" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F49" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="G49" s="19"/>
+      <c r="F49" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G49" s="7"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
@@ -3204,8 +3202,8 @@
         <v>34</v>
       </c>
       <c r="D50" s="19"/>
-      <c r="E50" s="19" t="s">
-        <v>113</v>
+      <c r="E50" s="20" t="s">
+        <v>88</v>
       </c>
       <c r="F50" s="19" t="s">
         <v>31</v>
@@ -3214,7 +3212,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="B51" s="19" t="s">
         <v>150</v>
@@ -3224,7 +3222,7 @@
       </c>
       <c r="D51" s="19"/>
       <c r="E51" s="19" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="F51" s="19" t="s">
         <v>31</v>
@@ -3233,7 +3231,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="B52" s="19" t="s">
         <v>150</v>
@@ -3243,7 +3241,7 @@
       </c>
       <c r="D52" s="19"/>
       <c r="E52" s="19" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="F52" s="19" t="s">
         <v>31</v>
@@ -3252,7 +3250,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="B53" s="19" t="s">
         <v>150</v>
@@ -3262,7 +3260,7 @@
       </c>
       <c r="D53" s="19"/>
       <c r="E53" s="19" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="F53" s="19" t="s">
         <v>31</v>
@@ -3281,7 +3279,7 @@
       </c>
       <c r="D54" s="19"/>
       <c r="E54" s="19" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="F54" s="19" t="s">
         <v>31</v>
@@ -3300,31 +3298,31 @@
       </c>
       <c r="D55" s="19"/>
       <c r="E55" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="F55" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G55" s="19"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="C56" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="F55" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="G55" s="19"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="B56" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="C56" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D56" s="28"/>
-      <c r="E56" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="F56" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="G56" s="28"/>
+      <c r="F56" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G56" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3334,10 +3332,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1424039-4C57-425F-8425-D8A336879F05}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3606,27 +3604,25 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="27" t="s">
-        <v>133</v>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -3793,12 +3789,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="beaba498-6342-4421-a18c-7bfd16d38d53" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4037,17 +4032,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="beaba498-6342-4421-a18c-7bfd16d38d53" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2275932-CD7C-4B19-A948-199D3E0E5FFC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9805D712-353E-429A-8628-FA34CABB75D5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="beaba498-6342-4421-a18c-7bfd16d38d53"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9e548fd3-f7b4-490c-9d07-36be117e6ce5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4072,18 +4077,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9805D712-353E-429A-8628-FA34CABB75D5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2275932-CD7C-4B19-A948-199D3E0E5FFC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="beaba498-6342-4421-a18c-7bfd16d38d53"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9e548fd3-f7b4-490c-9d07-36be117e6ce5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>